<commit_message>
v2.45 uni_uni updates to data_saver feature update to manual
</commit_message>
<xml_diff>
--- a/blueprints/components.xlsx
+++ b/blueprints/components.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\novak\PycharmProjects\pythonProject_LuxMeter\blueprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41449D5A-EE6B-4B85-908A-796C08721C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583F14B4-E7A5-4041-A00A-41DB99BE3DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>Raspberry Pi Pico</t>
   </si>
@@ -147,6 +139,21 @@
   </si>
   <si>
     <t>paměťová karta 16 GB již od</t>
+  </si>
+  <si>
+    <t>https://dratek.cz/arduino/121748-40-x-m-m-dupont-kabel-40-cm.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dratek.cz/arduino/121747-40-x-m-f-dupont-kabel-40-cm.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dratek.cz/arduino/1347-ssr-rele-modul-2-kanaly-5vdc-250vac-omron-g3mb-202p-solid-state-pro-arduino.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dratek.cz/arduino/122152-iic-i2c-oled-1-3-displej-128x64-modry.html </t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -182,12 +189,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -203,16 +216,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -496,7 +510,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -867,39 +883,87 @@
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
+      <c r="D30" s="3">
+        <v>2</v>
+      </c>
       <c r="E30" s="1"/>
+      <c r="F30" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
+      <c r="D31" s="3">
+        <v>2</v>
+      </c>
       <c r="E31" s="1"/>
+      <c r="F31" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
       <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
+      <c r="D33" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
+      <c r="D34" s="3">
+        <v>2</v>
+      </c>
       <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C35" s="1"/>
+      <c r="D35" s="3">
+        <v>2</v>
+      </c>
       <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
+      <c r="D36" s="3">
+        <v>2</v>
+      </c>
       <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C38" s="1"/>
+      <c r="D38" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E38" s="1"/>
+      <c r="F38" s="7" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -916,8 +980,16 @@
     <hyperlink ref="F18" r:id="rId11" xr:uid="{8FAF19D9-B2BE-4A87-BDE4-3EFB50DFB4F6}"/>
     <hyperlink ref="F25" r:id="rId12" xr:uid="{E0B75653-3365-4E21-AF51-AF093BBE55EE}"/>
     <hyperlink ref="F11" r:id="rId13" xr:uid="{6F9DD86E-9ADD-4F58-A110-491857CE284F}"/>
+    <hyperlink ref="F30" r:id="rId14" xr:uid="{B2E0AA2C-4E05-460F-8C6B-B99A768633F0}"/>
+    <hyperlink ref="F31" r:id="rId15" xr:uid="{A6EE51CA-7A9B-4C86-A75E-B93F71942A91}"/>
+    <hyperlink ref="F32" r:id="rId16" xr:uid="{2C54BC46-8A2A-41A8-9CF6-364CC052ABCC}"/>
+    <hyperlink ref="F33" r:id="rId17" xr:uid="{49A48A20-D097-4B71-9B50-2093369B97D1}"/>
+    <hyperlink ref="F34" r:id="rId18" xr:uid="{1F7B05E3-21ED-4A86-825D-8B1A909AA0B8}"/>
+    <hyperlink ref="F35" r:id="rId19" xr:uid="{2B8D9019-AEF5-4900-B9D7-29F645B23EF5}"/>
+    <hyperlink ref="F36" r:id="rId20" xr:uid="{8000C31C-AC29-4B70-8C0C-1F6EFA979DE1}"/>
+    <hyperlink ref="F38" r:id="rId21" xr:uid="{3C3A5EBA-142A-4A66-837D-1D9BC2719A36}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v2.46 uni_uni updates to data_saver feature change to SH1106 display
</commit_message>
<xml_diff>
--- a/blueprints/components.xlsx
+++ b/blueprints/components.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\novak\PycharmProjects\pythonProject_LuxMeter\blueprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583F14B4-E7A5-4041-A00A-41DB99BE3DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D681575B-8004-4C16-B48C-69C7D1338B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>Raspberry Pi Pico</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dratek.cz/arduino/7545-cinova-pajka-bezolovnata-100g-sn99-3cu0-7.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dratek.cz/arduino/1223-analogovy-multiplexer-16-kanalu-cd74hc4067.html </t>
   </si>
 </sst>
 </file>
@@ -508,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F38"/>
+  <dimension ref="A2:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,9 +966,47 @@
       <c r="D38" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="1"/>
+      <c r="E38" s="1">
+        <v>167</v>
+      </c>
       <c r="F38" s="7" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D39" s="3">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>350</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D41" s="3">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>27</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D42" s="3">
+        <v>9</v>
+      </c>
+      <c r="E42">
+        <v>67</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -988,8 +1032,11 @@
     <hyperlink ref="F35" r:id="rId19" xr:uid="{2B8D9019-AEF5-4900-B9D7-29F645B23EF5}"/>
     <hyperlink ref="F36" r:id="rId20" xr:uid="{8000C31C-AC29-4B70-8C0C-1F6EFA979DE1}"/>
     <hyperlink ref="F38" r:id="rId21" xr:uid="{3C3A5EBA-142A-4A66-837D-1D9BC2719A36}"/>
+    <hyperlink ref="F39" r:id="rId22" xr:uid="{9DD0A27C-CB73-4C05-A535-9FB8ED0353F5}"/>
+    <hyperlink ref="F41" r:id="rId23" xr:uid="{ABA9A2C2-6EC6-4C04-AC31-BAAB2CF4A3CB}"/>
+    <hyperlink ref="F42" r:id="rId24" xr:uid="{1746CC59-824F-4D27-8FAD-E52F93CB261D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update to 2.6 version of corridor programs
minor improvements to none in uni-uni
</commit_message>
<xml_diff>
--- a/blueprints/components.xlsx
+++ b/blueprints/components.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\novak\PycharmProjects\pythonProject_LuxMeter\blueprints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\novak\Documents\GitHub\LuxMeter\blueprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D681575B-8004-4C16-B48C-69C7D1338B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964F79AA-4B4B-4D3C-AD92-913EA27509D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,9 +123,6 @@
     <t>RTC hodiny reálného času</t>
   </si>
   <si>
-    <t>https://dratek.cz/arduino/842-rtc-hodiny-realneho-casu.html</t>
-  </si>
-  <si>
     <t>SPI Čtečka microSD karet</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://dratek.cz/arduino/1223-analogovy-multiplexer-16-kanalu-cd74hc4067.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dratek.cz/arduino/842-rtc-hodiny-realneho-casu.html </t>
   </si>
 </sst>
 </file>
@@ -169,7 +169,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#&quot; Kč&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +192,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -222,7 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -233,6 +240,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -516,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +584,7 @@
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="1">
@@ -626,12 +634,12 @@
         <v>61</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1">
         <v>20</v>
@@ -644,7 +652,7 @@
         <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -844,7 +852,7 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="1">
         <v>24</v>
@@ -857,12 +865,12 @@
         <v>24</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="1">
         <v>159</v>
@@ -894,7 +902,7 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
@@ -904,7 +912,7 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -920,7 +928,7 @@
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
       <c r="D33" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="7" t="s">
@@ -934,7 +942,7 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
@@ -954,7 +962,7 @@
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
@@ -964,13 +972,13 @@
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C38" s="1"/>
       <c r="D38" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E38" s="1">
         <v>167</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.25">
@@ -981,7 +989,7 @@
         <v>350</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
@@ -995,7 +1003,7 @@
         <v>27</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.25">
@@ -1035,8 +1043,9 @@
     <hyperlink ref="F39" r:id="rId22" xr:uid="{9DD0A27C-CB73-4C05-A535-9FB8ED0353F5}"/>
     <hyperlink ref="F41" r:id="rId23" xr:uid="{ABA9A2C2-6EC6-4C04-AC31-BAAB2CF4A3CB}"/>
     <hyperlink ref="F42" r:id="rId24" xr:uid="{1746CC59-824F-4D27-8FAD-E52F93CB261D}"/>
+    <hyperlink ref="F10" r:id="rId25" xr:uid="{BB10B99A-892D-4E3D-AB36-3519B1DA4B1B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId25"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>